<commit_message>
Removed raphidophytes from DFO2
</commit_message>
<xml_diff>
--- a/files/chem_compare_pelago.xlsx
+++ b/files/chem_compare_pelago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.belluz\Documents\R\calvert_spatial\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2305D51-9F02-4F25-B36E-D7D995FF1E86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3CE816-7929-4340-A600-D5F40F3AE50F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14604" xr2:uid="{F7E61890-90CC-4971-A6E8-850109A4A651}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4A1980-4DD6-4D64-ACD5-71D148C24D53}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1810,6 +1810,1336 @@
         <v>0.28678872187932331</v>
       </c>
     </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>43599</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>5.7323263958096504E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.22963124513626099</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.44158895810445148</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1.0570850074291229</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.90362678964932763</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.32898489137490589</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
+        <v>2.9817459583282471</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>43627</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2.8602246815959614E-2</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1.5667879255488515E-2</v>
+      </c>
+      <c r="F38" s="1">
+        <v>5.6313300932136672E-3</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.13635012010733286</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.2397773340344429</v>
+      </c>
+      <c r="J38" s="1">
+        <v>6.006661569699645E-3</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <v>3.1252996126810708</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>43652</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>9.5727333178122834E-2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.15508731951316199</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.31879934171835583</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.29948304841915768</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0.28024211774269742</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0.46228234966595966</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0</v>
+      </c>
+      <c r="L39" s="1">
+        <v>3.653606653213501</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>43682</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.32536328832308453</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.11616299673914909</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.66225416461626685</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.72082819541295373</v>
+      </c>
+      <c r="I40" s="1">
+        <v>1.0147175490856171</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0.26209647456804913</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1.0441686411698659</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>43710</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>5.6974166383345924E-2</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3.3338358819795153E-3</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.33215464651584625</v>
+      </c>
+      <c r="H41" s="1">
+        <v>2.9982023406773806E-2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.27503628780444461</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0.45692537724971771</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0</v>
+      </c>
+      <c r="L41" s="1">
+        <v>5.7756069501241045</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>43742</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3.3822124513487019E-2</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.36296539505322772</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0.43549260000387829</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0.18395648648341498</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.17954243719577789</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0.35560663044452667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>43955</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1.0050556622445583E-2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>7.0977946743369102E-2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2.2604870299498241E-2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2.3509274081637463E-3</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.14817456031839052</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0.10969635595877965</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.5430102298657099</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1">
+        <v>1.7768782575925191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2.8317473518351715E-2</v>
+      </c>
+      <c r="E44" s="1">
+        <v>5.961825574437777E-2</v>
+      </c>
+      <c r="F44" s="1">
+        <v>6.0880328218142189E-2</v>
+      </c>
+      <c r="G44" s="1">
+        <v>8.2155747960011169E-2</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.2548370435833931</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0.13114802290995917</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.26676763345797855</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0.46561978260676068</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1">
+        <v>6.068464989463488E-2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4.4205709050099053E-2</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>9.9396004031101867E-2</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.24043099830547968</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0.13972191140055656</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.12236608440677325</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1">
+        <v>0.48558686176935834</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2.8765986052652199E-2</v>
+      </c>
+      <c r="E46" s="1">
+        <v>6.8190089737375573E-2</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1.7109118149771045E-3</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.17826630175113678</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <v>5.6848062202334404E-2</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.15304492910703024</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1">
+        <v>1.7028066317240398</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>44079</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2.997131273150444E-2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2.771228055159251E-2</v>
+      </c>
+      <c r="F47" s="1">
+        <v>4.9933716278853053E-6</v>
+      </c>
+      <c r="G47" s="1">
+        <v>7.4860191593567535E-2</v>
+      </c>
+      <c r="H47" s="1">
+        <v>8.5111090292533234E-2</v>
+      </c>
+      <c r="I47" s="1">
+        <v>5.9116557861367859E-2</v>
+      </c>
+      <c r="J47" s="1">
+        <v>7.5090377281109497E-2</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0</v>
+      </c>
+      <c r="L47" s="1">
+        <v>0.20560710628827414</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>44108</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1">
+        <v>5.5066356047367053E-3</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2.7670164282123249E-2</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3.038213060547908E-2</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.12291522820790608</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.10001551111539204</v>
+      </c>
+      <c r="I48" s="1">
+        <v>7.4902457495530442E-2</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0.13215279330809912</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0</v>
+      </c>
+      <c r="L48" s="1">
+        <v>0.71864299972852075</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>43596</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>3.426308029641708E-2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>2.0540160747865837E-2</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.228759894768397</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.13405480111638704</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.46714912354946136</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.47159467140833539</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0.16919545084238052</v>
+      </c>
+      <c r="L49" s="1">
+        <v>3.4497001568476358</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>43626</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="1">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>4.8822063952684402E-2</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0.13173069804906845</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.21846549212932587</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0.15151063601175943</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0.25321843723456067</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0.28495572507381439</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0.17630474517742792</v>
+      </c>
+      <c r="L50" s="1">
+        <v>3.4038702249526978</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>43656</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>4.8960666482647262E-2</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <v>7.4592437595129013E-2</v>
+      </c>
+      <c r="G51" s="1">
+        <v>6.9429488852620125E-2</v>
+      </c>
+      <c r="H51" s="1">
+        <v>2.5868651088482391E-5</v>
+      </c>
+      <c r="I51" s="1">
+        <v>8.9574170609315232E-2</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0.26651046176751453</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0.15606223791837692</v>
+      </c>
+      <c r="L51" s="1">
+        <v>0.89684002598126733</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>43680</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.12882199759284654</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0.12192393342653911</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.11393118773897488</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0.1622543049355348</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0.25507856905460358</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0.15684353560209274</v>
+      </c>
+      <c r="K52" s="1">
+        <v>0.17425701022148132</v>
+      </c>
+      <c r="L52" s="1">
+        <v>0.50880299011866248</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>43709</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.15863658611973128</v>
+      </c>
+      <c r="E53" s="1">
+        <v>6.9431716576218605E-2</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0.21611339102188745</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.43155797819296521</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0.3087184528509776</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0.64217703541119897</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0.56963652372360229</v>
+      </c>
+      <c r="K53" s="1">
+        <v>1.4587849775950115</v>
+      </c>
+      <c r="L53" s="1">
+        <v>0.46956030279397964</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>43739</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2</v>
+      </c>
+      <c r="D54" s="1">
+        <v>4.8832381765047707E-2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3.5136038437485695E-2</v>
+      </c>
+      <c r="F54" s="1">
+        <v>2.852269106854995E-2</v>
+      </c>
+      <c r="G54" s="1">
+        <v>7.7427734931310013E-2</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0.11605968574682872</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0.12853609398007393</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0.10576246678829193</v>
+      </c>
+      <c r="K54" s="1">
+        <v>0.23940564940373102</v>
+      </c>
+      <c r="L54" s="1">
+        <v>3.5058327717706561E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1">
+        <v>8.9910125825554132E-3</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0.11415416250626247</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1.1145655977694939E-3</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0.1632093240817388</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0.13599417979518572</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0.36422852178414661</v>
+      </c>
+      <c r="K55" s="1">
+        <v>0</v>
+      </c>
+      <c r="L55" s="1">
+        <v>8.4786914189656581</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="1">
+        <v>2</v>
+      </c>
+      <c r="D56" s="1">
+        <v>6.2298837428291641E-2</v>
+      </c>
+      <c r="E56" s="1">
+        <v>4.5084602509935699E-2</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0.14455142120520273</v>
+      </c>
+      <c r="H56" s="1">
+        <v>9.571799387534459E-2</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0.23999580989281336</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0.2148365949591001</v>
+      </c>
+      <c r="K56" s="1">
+        <v>0</v>
+      </c>
+      <c r="L56" s="1">
+        <v>1.9644079407056172</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.13798973833521208</v>
+      </c>
+      <c r="E57" s="1">
+        <v>6.907259502137701E-3</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1.5466086430630337E-3</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0.2367029438416163</v>
+      </c>
+      <c r="H57" s="1">
+        <v>9.102491894736886E-4</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0.36847875515619916</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0.24937747418880463</v>
+      </c>
+      <c r="K57" s="1">
+        <v>0</v>
+      </c>
+      <c r="L57" s="1">
+        <v>4.6901398499806719</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2</v>
+      </c>
+      <c r="D58" s="1">
+        <v>4.7243334973851837E-2</v>
+      </c>
+      <c r="E58" s="1">
+        <v>6.2143117189407349E-2</v>
+      </c>
+      <c r="F58" s="1">
+        <v>6.9407061363259956E-2</v>
+      </c>
+      <c r="G58" s="1">
+        <v>8.7692101796468094E-2</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1.8064523659025629E-3</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0.14076162253816923</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0.18976708253224692</v>
+      </c>
+      <c r="K58" s="1">
+        <v>0.19836195806662241</v>
+      </c>
+      <c r="L58" s="1">
+        <v>2.4026165008544922</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1">
+        <v>4.9704677114884056E-2</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4.6047393853465714E-2</v>
+      </c>
+      <c r="F59" s="1">
+        <v>5.7832344124714531E-2</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0.12209140509366989</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0.15603229279319444</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0.17373295873403549</v>
+      </c>
+      <c r="J59" s="1">
+        <v>0.14393153786659241</v>
+      </c>
+      <c r="K59" s="1">
+        <v>0</v>
+      </c>
+      <c r="L59" s="1">
+        <v>0.7726530830065409</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="1">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1">
+        <v>2.9435679316520691E-2</v>
+      </c>
+      <c r="E60" s="1">
+        <v>4.5386812960108124E-2</v>
+      </c>
+      <c r="F60" s="1">
+        <v>4.4409139702717461E-2</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0.14358566577235857</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0.10439598808685939</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0.18934048463900885</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0.3099943995475769</v>
+      </c>
+      <c r="K60" s="1">
+        <v>0</v>
+      </c>
+      <c r="L60" s="1">
+        <v>0.9983908633391062</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>43598</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.3713095982869466</v>
+      </c>
+      <c r="E61" s="1">
+        <v>6.2635176194210844E-3</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0.26218534260988235</v>
+      </c>
+      <c r="H61" s="1">
+        <v>6.8260605136553443E-4</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0.33303802708784741</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1">
+        <v>0</v>
+      </c>
+      <c r="L61" s="1">
+        <v>11.183916886647543</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>43625</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <v>4.1713184987505279E-2</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0.10321928312381108</v>
+      </c>
+      <c r="G62" s="1">
+        <v>8.3280516788363457E-2</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0.1334383524954319</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0.11105391134818395</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0.20988628019889197</v>
+      </c>
+      <c r="K62" s="1">
+        <v>0.16846386591593424</v>
+      </c>
+      <c r="L62" s="1">
+        <v>1.9359140594800313</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>43653</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1">
+        <v>9.6862968057394028E-2</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0.23883150269587836</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0.1921005348364512</v>
+      </c>
+      <c r="H63" s="1">
+        <v>4.709719990690549E-4</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.2260843813419342</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0.50952098270257318</v>
+      </c>
+      <c r="K63" s="1">
+        <v>0.19850883136192957</v>
+      </c>
+      <c r="L63" s="1">
+        <v>3.2964237133661904</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>43683</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="1">
+        <v>2</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.1552652046084404</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0.43088962137699127</v>
+      </c>
+      <c r="G64" s="1">
+        <v>9.3417612845466166E-2</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0.4408913527925809</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0.25195166220267612</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0.58068067332108819</v>
+      </c>
+      <c r="K64" s="1">
+        <v>0.25170752654472989</v>
+      </c>
+      <c r="L64" s="1">
+        <v>3.0096037785212197</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>43708</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2</v>
+      </c>
+      <c r="D65" s="1">
+        <v>9.2524251590172454E-2</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0.38380198180675507</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0.42227564255396527</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0.46941063801447552</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0.27222381780544919</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0.75459482272466027</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0.88896942138671875</v>
+      </c>
+      <c r="K65" s="1">
+        <v>0.78173213203748071</v>
+      </c>
+      <c r="L65" s="1">
+        <v>0.76122228304545081</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>43743</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="1">
+        <v>2</v>
+      </c>
+      <c r="D66" s="1">
+        <v>5.0385082761446633E-2</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0.15629815434416136</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0.23062742004791895</v>
+      </c>
+      <c r="G66" s="1">
+        <v>6.6957105261584118E-2</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0.14188076307376227</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0.22673077632983527</v>
+      </c>
+      <c r="J66" s="1">
+        <v>0.22211085756619772</v>
+      </c>
+      <c r="K66" s="1">
+        <v>0.1942227284113566</v>
+      </c>
+      <c r="L66" s="1">
+        <v>0.64285404483477271</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0.10578483467300732</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1.2212992684605222E-3</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0.10915662224094073</v>
+      </c>
+      <c r="H67" s="1">
+        <v>1.6320268623530865E-3</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0.10851028685768445</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0.28999344011147815</v>
+      </c>
+      <c r="K67" s="1">
+        <v>0</v>
+      </c>
+      <c r="L67" s="1">
+        <v>4.4214761257171631</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="1">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1">
+        <v>4.2052078992128372E-2</v>
+      </c>
+      <c r="E68" s="1">
+        <v>3.6347233069439731E-2</v>
+      </c>
+      <c r="F68" s="1">
+        <v>4.6850280836224556E-2</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0.10914688060681026</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0.1305042083064715</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0.15945560733477274</v>
+      </c>
+      <c r="J68" s="1">
+        <v>0.21388613184293112</v>
+      </c>
+      <c r="K68" s="1">
+        <v>0</v>
+      </c>
+      <c r="L68" s="1">
+        <v>1.6277880072593689</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>44017</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="1">
+        <v>2</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.11422773078083992</v>
+      </c>
+      <c r="E69" s="1">
+        <v>7.6206081236402198E-2</v>
+      </c>
+      <c r="F69" s="1">
+        <v>7.285125999866674E-4</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0.16866081332166991</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0.2023045631746451</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0.21082696815331778</v>
+      </c>
+      <c r="J69" s="1">
+        <v>0.22153590122858682</v>
+      </c>
+      <c r="K69" s="1">
+        <v>0.12607067575057349</v>
+      </c>
+      <c r="L69" s="1">
+        <v>2.8680478731791177</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="1">
+        <v>2</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0.26261752595504123</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0.14942513157924017</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0.23481451223293939</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0.2240930919845899</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0.37658547610044479</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0.32377645373344421</v>
+      </c>
+      <c r="J70" s="1">
+        <v>0.2081861843665441</v>
+      </c>
+      <c r="K70" s="1">
+        <v>0.34956898788611096</v>
+      </c>
+      <c r="L70" s="1">
+        <v>4.568633002539476E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>44106</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2</v>
+      </c>
+      <c r="D71" s="1">
+        <v>2.7839865845938522E-2</v>
+      </c>
+      <c r="E71" s="1">
+        <v>4.7892979656656585E-2</v>
+      </c>
+      <c r="F71" s="1">
+        <v>3.8082009181380272E-2</v>
+      </c>
+      <c r="G71" s="1">
+        <v>5.0482298557957016E-2</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0.11085083708167076</v>
+      </c>
+      <c r="I71" s="1">
+        <v>8.5060006628433868E-2</v>
+      </c>
+      <c r="J71" s="1">
+        <v>0.14948464805881181</v>
+      </c>
+      <c r="K71" s="1">
+        <v>0</v>
+      </c>
+      <c r="L71" s="1">
+        <v>0.30600252747535706</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>